<commit_message>
Alteraçoes na GUI da aplicaçao
</commit_message>
<xml_diff>
--- a/Enviar.xlsx
+++ b/Enviar.xlsx
@@ -37,7 +37,7 @@
     <t>te</t>
   </si>
   <si>
-    <t>Weslao</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -45,7 +45,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,12 +56,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -99,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -107,10 +101,16 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -430,9 +430,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -469,190 +469,156 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="22.5">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="22.5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="22.5">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="22.5">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="22.5">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="22.5">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="22.5">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="22.5">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="22.5">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="22.5">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="22.5">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
+      <c r="A14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="22.5">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
+      <c r="A15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="22.5">
-      <c r="A16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
+      <c r="A16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="22.5">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
+      <c r="A17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="22.5">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
+      <c r="A18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2">
-        <v>553134127713</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
+      <c r="A19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="22.5">
-      <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2">
-        <v>5531984683539</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
+      <c r="A20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>